<commit_message>
1. Initialised excel and cim docs.
</commit_message>
<xml_diff>
--- a/cmip6/models/norcpm1/cmip6_ncc_norcpm1_aerosol.xlsx
+++ b/cmip6/models/norcpm1/cmip6_ncc_norcpm1_aerosol.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="503">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -162,6 +162,9 @@
     <t>cmip6.aerosol.key_properties.name</t>
   </si>
   <si>
+    <t>NorESM-aerosol</t>
+  </si>
+  <si>
     <t>1.1.1.2 *</t>
   </si>
   <si>
@@ -207,6 +210,9 @@
     <t>cmip6.aerosol.key_properties.scheme_scope</t>
   </si>
   <si>
+    <t>Troposphere</t>
+  </si>
+  <si>
     <t>troposphere</t>
   </si>
   <si>
@@ -234,6 +240,9 @@
     <t>cmip6.aerosol.key_properties.basic_approximations</t>
   </si>
   <si>
+    <t>A modal-process-bin approximation</t>
+  </si>
+  <si>
     <t>1.1.1.6 *</t>
   </si>
   <si>
@@ -975,6 +984,10 @@
     <t>cmip6.aerosol.concentrations.overview</t>
   </si>
   <si>
+    <t>Description: Emissions for the sulphur cycle include emissions of sulphate aerosol precursors: sulphur dioxide and dimethylsulphide in addition to SO4 formed close to the emissions source( 2%).  For sulphur dioxide and SO4, anthropogenic and biomass burning emissions are taken from Lamarque et al. (2009). Natural emissions from volcanoes are provided as a 3D field. (Dentener et al., 2006) DMS emissions have no interannual variation, and  are taken from the day by day varying dataset from the year 2000 in Dentener et al. (2006).  All sulphur-cycle emissions are expressed in term of mass of sulphur within the model. For black-carbon and organic-carbon aerosols from fossil-fuel and biofuel emissions, emissions are provided at the two lowest model layers, following the classification in Dentener et al. 2006 together with the source classification in Lamarque et al (2009). For biomass-burning aerosol, emissions are provided from Lamarque et al. (2009) and distributed vertically as in Dentener et al. (2006). The climatology of monthly-averaged mass-mixing ratios of secondary organic aerosol from terpene emissions are taken from Dentener et al. (2006), but scaled to the total numbers in Hoyle et al. (2007). Primary organic matter from the ocean is parameterised by using the fine mode sea-salt emissions in Dentener et al. (2006) scaled to the number given in Spracklen et al. (2008). Emissions of organic carbon aerosols are expressed in term of mass of total organic matter._x000D_
+Emissions from mineral dust are based on the year 2000 calculated in Dentener et al. (2006). Sea-salt aerosol emissions are computed interactively depending on modelled near-surface wind speeds and sea-surface temperatures (Struthers et al., 2011). All emission fields except DMS and dust are provided as monthly means, which are read in at the beginning of each moth. DMS and mineral dust are given as daily values, although with no interannual variation</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.1.1.3 </t>
   </si>
   <si>
@@ -987,6 +1000,9 @@
     <t>cmip6.aerosol.concentrations.prescribed_lower_boundary</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.1.1.4 </t>
   </si>
   <si>
@@ -999,6 +1015,9 @@
     <t>cmip6.aerosol.concentrations.prescribed_upper_boundary</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.1.1.5 </t>
   </si>
   <si>
@@ -1323,6 +1342,9 @@
     <t>cmip6.aerosol.model.overview</t>
   </si>
   <si>
+    <t>Background (primary) aerosol size modes are assumed to be log-normally distributed and have constant median radii and standard deviations at the point of emission. The size distributions for modified aerosol modes, after growth, are not restricted to log-normality. Although the modified aerosol size distributions are not calculated from "first principles" in the model itself, as in a sectional model, modal size parameters (for droplet activation and subsequent indirect effects) and aerosol optical properties (for the direct effect) are found from look-up tables (by interpolation in up to 5 dimensions) of values which have been computed with a separate code which takes into account growth by condensation (including hygroscopic growth), coagulation and wet-phase chemistry/cloud processing. These tables have been made for a large array of different input values for the amount of condensation, coagulation etc (relative to a background aerosol) for the various constituents.</t>
+  </si>
+  <si>
     <t>7.1.1.3 *</t>
   </si>
   <si>
@@ -1335,6 +1357,9 @@
     <t>cmip6.aerosol.model.processes</t>
   </si>
   <si>
+    <t>Advection (horizontal)</t>
+  </si>
+  <si>
     <t>Dry deposition</t>
   </si>
   <si>
@@ -1362,9 +1387,6 @@
     <t>Ageing</t>
   </si>
   <si>
-    <t>Advection (horizontal)</t>
-  </si>
-  <si>
     <t>Advection (vertical)</t>
   </si>
   <si>
@@ -1386,15 +1408,15 @@
     <t>cmip6.aerosol.model.coupling</t>
   </si>
   <si>
+    <t>Clouds</t>
+  </si>
+  <si>
     <t>Radiation</t>
   </si>
   <si>
     <t>Land surface</t>
   </si>
   <si>
-    <t>Clouds</t>
-  </si>
-  <si>
     <t>Ocean</t>
   </si>
   <si>
@@ -1402,6 +1424,9 @@
   </si>
   <si>
     <t>Gas phase chemistry</t>
+  </si>
+  <si>
+    <t>Other: landsurface</t>
   </si>
   <si>
     <t>7.1.1.5 *</t>
@@ -2280,14 +2305,16 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -2295,15 +2322,15 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
@@ -2311,10 +2338,10 @@
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -2322,15 +2349,15 @@
         <v>43</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="178" customHeight="1">
@@ -2338,21 +2365,21 @@
     </row>
     <row r="18" spans="1:31" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="24" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="24" customHeight="1">
@@ -2361,29 +2388,31 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="24" customHeight="1">
-      <c r="B21" s="11"/>
+      <c r="B21" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="AA21" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AB21" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AC21" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AE21" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="24" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="24" customHeight="1">
@@ -2391,32 +2420,34 @@
         <v>43</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="27" spans="1:31" ht="24" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="24" customHeight="1">
       <c r="A28" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:31" ht="24" customHeight="1">
@@ -2425,80 +2456,86 @@
       </c>
     </row>
     <row r="30" spans="1:31" ht="24" customHeight="1">
-      <c r="B30" s="11"/>
+      <c r="B30" s="11" t="s">
+        <v>77</v>
+      </c>
       <c r="AA30" s="6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AB30" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AC30" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:31" ht="24" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="A33" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
-      <c r="B34" s="11"/>
+      <c r="B34" s="11">
+        <v>20</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="24" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
-      <c r="B38" s="11"/>
+      <c r="B38" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
       <c r="A41" s="12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="24" customHeight="1">
       <c r="B42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="24" customHeight="1">
@@ -2506,10 +2543,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="24" customHeight="1">
@@ -2517,10 +2554,10 @@
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:30" ht="24" customHeight="1">
@@ -2528,10 +2565,10 @@
         <v>43</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:30" ht="24" customHeight="1">
@@ -2539,10 +2576,10 @@
     </row>
     <row r="52" spans="1:30" ht="24" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="24" customHeight="1">
@@ -2550,15 +2587,15 @@
         <v>43</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:30" ht="24" customHeight="1">
       <c r="B54" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="24" customHeight="1">
@@ -2566,68 +2603,70 @@
     </row>
     <row r="58" spans="1:30" ht="24" customHeight="1">
       <c r="A58" s="12" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:30" ht="24" customHeight="1">
       <c r="B59" s="13" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:30" ht="24" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:30" ht="24" customHeight="1">
       <c r="A62" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:30" ht="24" customHeight="1">
-      <c r="B63" s="11"/>
+      <c r="B63" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="AA63" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="AB63" s="6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AC63" s="6" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AD63" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:35" ht="24" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:35" ht="24" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:35" ht="24" customHeight="1">
@@ -2635,21 +2674,21 @@
     </row>
     <row r="69" spans="1:35" ht="24" customHeight="1">
       <c r="A69" s="9" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:35" ht="24" customHeight="1">
       <c r="A70" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:35" ht="24" customHeight="1">
@@ -2657,21 +2696,21 @@
     </row>
     <row r="73" spans="1:35" ht="24" customHeight="1">
       <c r="A73" s="9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:35" ht="24" customHeight="1">
       <c r="A74" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:35" ht="24" customHeight="1">
@@ -2679,59 +2718,59 @@
     </row>
     <row r="77" spans="1:35" ht="24" customHeight="1">
       <c r="A77" s="9" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:35" ht="24" customHeight="1">
       <c r="A78" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:35" ht="24" customHeight="1">
       <c r="B79" s="11"/>
       <c r="AA79" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AB79" s="6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AC79" s="6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AD79" s="6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AE79" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AF79" s="6" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AG79" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AH79" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AI79" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="24" customHeight="1">
       <c r="A82" s="12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="24" customHeight="1">
@@ -2739,10 +2778,10 @@
     </row>
     <row r="85" spans="1:3" ht="24" customHeight="1">
       <c r="A85" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="24" customHeight="1">
@@ -2750,15 +2789,15 @@
         <v>43</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="24" customHeight="1">
       <c r="B87" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="24" customHeight="1">
@@ -2766,10 +2805,10 @@
     </row>
     <row r="90" spans="1:3" ht="24" customHeight="1">
       <c r="A90" s="9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="24" customHeight="1">
@@ -2777,15 +2816,15 @@
         <v>43</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="24" customHeight="1">
       <c r="B92" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
@@ -2793,21 +2832,21 @@
     </row>
     <row r="95" spans="1:3" ht="24" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="24" customHeight="1">
       <c r="A96" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="24" customHeight="1">
@@ -2815,20 +2854,20 @@
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1">
       <c r="A100" s="12" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
       <c r="B101" s="13" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
       <c r="A103" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B103" s="9" t="s">
         <v>42</v>
@@ -2839,10 +2878,10 @@
         <v>43</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
@@ -2850,10 +2889,10 @@
     </row>
     <row r="107" spans="1:3" ht="24" customHeight="1">
       <c r="A107" s="9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="24" customHeight="1">
@@ -2861,10 +2900,10 @@
         <v>43</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="24" customHeight="1">
@@ -2872,21 +2911,21 @@
     </row>
     <row r="111" spans="1:3" ht="24" customHeight="1">
       <c r="A111" s="9" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1">
       <c r="A112" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="24" customHeight="1">
@@ -2894,21 +2933,21 @@
     </row>
     <row r="115" spans="1:3" ht="24" customHeight="1">
       <c r="A115" s="9" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="24" customHeight="1">
       <c r="A116" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="24" customHeight="1">
@@ -2916,21 +2955,21 @@
     </row>
     <row r="119" spans="1:3" ht="24" customHeight="1">
       <c r="A119" s="9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="24" customHeight="1">
       <c r="A120" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1">
@@ -2938,23 +2977,23 @@
     </row>
     <row r="124" spans="1:3" ht="24" customHeight="1">
       <c r="A124" s="12" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="24" customHeight="1">
       <c r="B125" s="13" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="24" customHeight="1">
       <c r="A127" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="24" customHeight="1">
@@ -2962,15 +3001,15 @@
         <v>43</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="24" customHeight="1">
       <c r="B129" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="178" customHeight="1">
@@ -2978,10 +3017,10 @@
     </row>
     <row r="132" spans="1:3" ht="24" customHeight="1">
       <c r="A132" s="9" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="24" customHeight="1">
@@ -2989,15 +3028,15 @@
         <v>43</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
       <c r="B134" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="24" customHeight="1">
@@ -3005,10 +3044,10 @@
     </row>
     <row r="137" spans="1:3" ht="24" customHeight="1">
       <c r="A137" s="9" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="24" customHeight="1">
@@ -3016,15 +3055,15 @@
         <v>43</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1">
       <c r="B139" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="24" customHeight="1">
@@ -3032,10 +3071,10 @@
     </row>
     <row r="142" spans="1:3" ht="24" customHeight="1">
       <c r="A142" s="9" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="24" customHeight="1">
@@ -3043,15 +3082,15 @@
         <v>43</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1">
       <c r="B144" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="24" customHeight="1">
@@ -3119,20 +3158,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -3143,10 +3182,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -3154,10 +3193,10 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -3165,15 +3204,15 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
@@ -3181,21 +3220,21 @@
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
@@ -3203,20 +3242,20 @@
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
       <c r="B19" s="13" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>42</v>
@@ -3227,10 +3266,10 @@
         <v>43</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
@@ -3238,10 +3277,10 @@
     </row>
     <row r="25" spans="1:3" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="24" customHeight="1">
@@ -3249,10 +3288,10 @@
         <v>43</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="24" customHeight="1">
@@ -3260,21 +3299,21 @@
     </row>
     <row r="29" spans="1:3" ht="24" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="24" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" customHeight="1">
@@ -3282,21 +3321,21 @@
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
       <c r="A34" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
@@ -3304,21 +3343,21 @@
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
       <c r="A38" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
@@ -3359,20 +3398,20 @@
   <sheetData>
     <row r="1" spans="1:31" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -3383,10 +3422,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="24" customHeight="1">
@@ -3394,10 +3433,10 @@
     </row>
     <row r="8" spans="1:31" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="24" customHeight="1">
@@ -3405,15 +3444,15 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="178" customHeight="1">
@@ -3421,58 +3460,58 @@
     </row>
     <row r="13" spans="1:31" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="24" customHeight="1">
       <c r="B15" s="11"/>
       <c r="AA15" s="6" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AB15" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AC15" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="AD15" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AE15" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="24" customHeight="1">
@@ -3483,38 +3522,38 @@
     <row r="20" spans="1:31" ht="24" customHeight="1">
       <c r="B20" s="11"/>
       <c r="AA20" s="6" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AB20" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="AC20" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="AD20" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="AE20" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="24" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="24" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="24" customHeight="1">
@@ -3525,16 +3564,16 @@
     <row r="25" spans="1:31" ht="24" customHeight="1">
       <c r="B25" s="11"/>
       <c r="AA25" s="6" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="AD25" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3569,20 +3608,20 @@
   <sheetData>
     <row r="1" spans="1:33" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -3593,10 +3632,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="24" customHeight="1">
@@ -3604,10 +3643,10 @@
     </row>
     <row r="8" spans="1:33" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="24" customHeight="1">
@@ -3615,15 +3654,15 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="178" customHeight="1">
@@ -3631,21 +3670,21 @@
     </row>
     <row r="13" spans="1:33" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="24" customHeight="1">
@@ -3656,44 +3695,44 @@
     <row r="16" spans="1:33" ht="24" customHeight="1">
       <c r="B16" s="11"/>
       <c r="AA16" s="6" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="AB16" s="6" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="AC16" s="6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="AD16" s="6" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="AE16" s="6" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="AF16" s="6" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="AG16" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:35" ht="24" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="24" customHeight="1">
@@ -3704,76 +3743,76 @@
     <row r="21" spans="1:35" ht="24" customHeight="1">
       <c r="B21" s="11"/>
       <c r="AA21" s="6" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="AB21" s="6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="AC21" s="6" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="AE21" s="6" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="AF21" s="6" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="AG21" s="6" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AH21" s="6" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="AI21" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="24" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="24" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:35" ht="24" customHeight="1">
       <c r="B25" s="11"/>
       <c r="AA25" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="AD25" s="6" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="AE25" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:35" ht="24" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="24" customHeight="1">
@@ -3781,15 +3820,15 @@
         <v>43</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="24" customHeight="1">
       <c r="B29" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="24" customHeight="1">
@@ -3797,10 +3836,10 @@
     </row>
     <row r="32" spans="1:35" ht="24" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
@@ -3808,15 +3847,15 @@
         <v>43</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
       <c r="B34" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
@@ -3824,10 +3863,10 @@
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
@@ -3835,15 +3874,15 @@
         <v>43</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
       <c r="B39" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="24" customHeight="1">
@@ -3851,10 +3890,10 @@
     </row>
     <row r="42" spans="1:3" ht="24" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
@@ -3862,15 +3901,15 @@
         <v>43</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1">
       <c r="B44" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="24" customHeight="1">
@@ -3878,10 +3917,10 @@
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1">
       <c r="A47" s="9" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
@@ -3889,10 +3928,10 @@
         <v>43</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="24" customHeight="1">
@@ -3930,20 +3969,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -3954,10 +3993,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -3965,10 +4004,10 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -3976,26 +4015,28 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -4003,26 +4044,28 @@
         <v>43</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="24" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
@@ -4030,26 +4073,28 @@
         <v>43</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1">
       <c r="B20" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1">
-      <c r="B21" s="11"/>
+      <c r="B21" s="11" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="24" customHeight="1">
@@ -4057,15 +4102,15 @@
         <v>43</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="24" customHeight="1">
       <c r="B25" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="24" customHeight="1">
@@ -4073,10 +4118,10 @@
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="24" customHeight="1">
@@ -4084,15 +4129,15 @@
         <v>43</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="24" customHeight="1">
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" customHeight="1">
@@ -4119,20 +4164,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -4143,10 +4188,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -4154,10 +4199,10 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -4165,15 +4210,15 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
@@ -4181,34 +4226,34 @@
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
@@ -4216,21 +4261,21 @@
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
@@ -4238,21 +4283,21 @@
     </row>
     <row r="25" spans="1:3" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="24" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="24" customHeight="1">
@@ -4260,10 +4305,10 @@
     </row>
     <row r="30" spans="1:3" ht="24" customHeight="1">
       <c r="A30" s="12" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" customHeight="1">
@@ -4271,21 +4316,21 @@
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
       <c r="A34" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
@@ -4293,21 +4338,21 @@
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
       <c r="A38" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
@@ -4315,10 +4360,10 @@
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="24" customHeight="1">
@@ -4326,10 +4371,10 @@
         <v>43</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
@@ -4337,34 +4382,34 @@
     </row>
     <row r="46" spans="1:3" ht="24" customHeight="1">
       <c r="A46" s="12" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1">
       <c r="B47" s="13" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="24" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="24" customHeight="1">
       <c r="A50" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="24" customHeight="1">
@@ -4372,21 +4417,21 @@
     </row>
     <row r="53" spans="1:3" ht="24" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="24" customHeight="1">
       <c r="A54" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="24" customHeight="1">
@@ -4394,21 +4439,21 @@
     </row>
     <row r="57" spans="1:3" ht="24" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="24" customHeight="1">
       <c r="A58" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="24" customHeight="1">
@@ -4416,23 +4461,23 @@
     </row>
     <row r="62" spans="1:3" ht="24" customHeight="1">
       <c r="A62" s="12" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="24" customHeight="1">
       <c r="B63" s="13" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="24" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="24" customHeight="1">
@@ -4440,15 +4485,15 @@
         <v>43</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="24" customHeight="1">
       <c r="B67" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="178" customHeight="1">
@@ -4456,21 +4501,21 @@
     </row>
     <row r="70" spans="1:3" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="24" customHeight="1">
       <c r="A71" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="24" customHeight="1">
@@ -4478,21 +4523,21 @@
     </row>
     <row r="74" spans="1:3" ht="24" customHeight="1">
       <c r="A74" s="9" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="24" customHeight="1">
       <c r="A75" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="24" customHeight="1">
@@ -4500,23 +4545,23 @@
     </row>
     <row r="79" spans="1:3" ht="24" customHeight="1">
       <c r="A79" s="12" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="24" customHeight="1">
       <c r="B80" s="13" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="24" customHeight="1">
       <c r="A82" s="9" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="24" customHeight="1">
@@ -4524,15 +4569,15 @@
         <v>43</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="24" customHeight="1">
       <c r="B84" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="178" customHeight="1">
@@ -4540,21 +4585,21 @@
     </row>
     <row r="87" spans="1:3" ht="24" customHeight="1">
       <c r="A87" s="9" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="24" customHeight="1">
       <c r="A88" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="24" customHeight="1">
@@ -4562,21 +4607,21 @@
     </row>
     <row r="91" spans="1:3" ht="24" customHeight="1">
       <c r="A91" s="9" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="24" customHeight="1">
       <c r="A92" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
@@ -4584,21 +4629,21 @@
     </row>
     <row r="95" spans="1:3" ht="24" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="24" customHeight="1">
       <c r="A96" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="24" customHeight="1">
@@ -4606,21 +4651,21 @@
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
       <c r="A99" s="9" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1">
       <c r="A100" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
@@ -4628,21 +4673,21 @@
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
       <c r="A103" s="9" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="24" customHeight="1">
       <c r="A104" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
@@ -4705,7 +4750,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD36"/>
+  <dimension ref="A1:XFD48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4719,7 +4764,7 @@
   <sheetData>
     <row r="1" spans="1:39" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>5</v>
@@ -4727,12 +4772,12 @@
     </row>
     <row r="2" spans="1:39" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -4743,10 +4788,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="24" customHeight="1">
@@ -4754,10 +4799,10 @@
     </row>
     <row r="8" spans="1:39" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:39" ht="24" customHeight="1">
@@ -4765,37 +4810,39 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:39" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="13" spans="1:39" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
     </row>
     <row r="14" spans="1:39" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:39" ht="24" customHeight="1">
@@ -4804,276 +4851,804 @@
       </c>
     </row>
     <row r="16" spans="1:39" ht="24" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>444</v>
+      </c>
       <c r="AA16" s="6" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="AB16" s="6" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="AC16" s="6" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="AD16" s="6" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="AE16" s="6" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="AF16" s="6" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="AG16" s="6" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="AH16" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI16" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ16" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="AI16" s="6" t="s">
+      <c r="AK16" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL16" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM16" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="24" customHeight="1">
+      <c r="B17" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA17" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="AJ16" s="6" t="s">
+      <c r="AB17" s="6" t="s">
         <v>446</v>
       </c>
-      <c r="AK16" s="6" t="s">
+      <c r="AC17" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="AL16" s="6" t="s">
+      <c r="AD17" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="AM16" s="6" t="s">
+      <c r="AE17" s="6" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="18" spans="1:35" ht="24" customHeight="1">
-      <c r="A18" s="9" t="s">
+      <c r="AF17" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="AG17" s="6" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="19" spans="1:35" ht="24" customHeight="1">
-      <c r="A19" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="AH17" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="AI17" s="6" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="20" spans="1:35" ht="24" customHeight="1">
-      <c r="B20" s="10" t="s">
+      <c r="AJ17" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL17" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM17" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" ht="24" customHeight="1">
+      <c r="B18" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="AA18" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB18" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC18" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF18" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AG18" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AH18" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI18" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ18" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK18" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL18" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM18" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" ht="24" customHeight="1">
+      <c r="B19" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="AA19" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB19" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC19" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF19" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AG19" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AH19" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI19" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ19" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK19" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL19" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM19" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" ht="24" customHeight="1">
+      <c r="B20" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="AA20" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC20" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD20" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE20" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF20" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AH20" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI20" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ20" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK20" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL20" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM20" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" ht="24" customHeight="1">
+      <c r="B21" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE21" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF21" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AG21" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AH21" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI21" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ21" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK21" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL21" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM21" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="24" customHeight="1">
+      <c r="B22" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB22" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC22" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF22" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AG22" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AH22" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI22" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ22" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK22" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL22" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM22" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" ht="24" customHeight="1">
+      <c r="B23" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="AA23" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB23" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC23" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE23" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF23" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AG23" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI23" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ23" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK23" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL23" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM23" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="24" customHeight="1">
+      <c r="B24" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="AA24" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB24" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC24" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD24" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE24" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF24" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AG24" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AH24" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI24" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ24" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK24" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL24" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM24" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="24" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC25" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE25" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF25" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AG25" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AI25" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ25" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AK25" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL25" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AM25" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" ht="24" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" ht="24" customHeight="1">
+      <c r="A28" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" ht="24" customHeight="1">
+      <c r="B29" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="24" customHeight="1">
-      <c r="B21" s="11"/>
-      <c r="AA21" s="6" t="s">
-        <v>454</v>
-      </c>
-      <c r="AB21" s="6" t="s">
+    <row r="30" spans="1:39" ht="24" customHeight="1">
+      <c r="B30" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="AA30" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="AB30" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="AC30" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="AC21" s="6" t="s">
-        <v>448</v>
-      </c>
-      <c r="AD21" s="6" t="s">
-        <v>456</v>
-      </c>
-      <c r="AE21" s="6" t="s">
-        <v>457</v>
-      </c>
-      <c r="AF21" s="6" t="s">
-        <v>458</v>
-      </c>
-      <c r="AG21" s="6" t="s">
-        <v>459</v>
-      </c>
-      <c r="AH21" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>460</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="AD30" s="6" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
-      <c r="A24" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="AE30" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AF30" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="AG30" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="AH30" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" ht="24" customHeight="1">
+      <c r="B31" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="AA31" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="AB31" s="6" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="25" spans="1:35" ht="24" customHeight="1">
-      <c r="B25" s="10" t="s">
+      <c r="AC31" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AD31" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="AE31" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AF31" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="AG31" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="AH31" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" ht="24" customHeight="1">
+      <c r="B32" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="AA32" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="AB32" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="AC32" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AD32" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="AE32" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AF32" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="AG32" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="AH32" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:40" ht="24" customHeight="1">
+      <c r="A34" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40" ht="24" customHeight="1">
+      <c r="A35" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" ht="24" customHeight="1">
+      <c r="B36" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="24" customHeight="1">
-      <c r="B26" s="11"/>
-      <c r="AA26" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="AB26" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="AC26" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="AD26" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="AE26" s="6" t="s">
-        <v>468</v>
-      </c>
-      <c r="AF26" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="AG26" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="AH26" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AI26" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:35" ht="24" customHeight="1">
-      <c r="A28" s="9" t="s">
+    <row r="37" spans="1:40" ht="24" customHeight="1">
+      <c r="B37" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="AA37" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AB37" s="6" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="29" spans="1:35" ht="24" customHeight="1">
-      <c r="A29" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="10" t="s">
+      <c r="AC37" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="AD37" s="6" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="30" spans="1:35" ht="24" customHeight="1">
-      <c r="B30" s="10" t="s">
+      <c r="AE37" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AF37" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AG37" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AH37" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AI37" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:40" ht="24" customHeight="1">
+      <c r="B38" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="AA38" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AB38" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AC38" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD38" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AE38" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AF38" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AG38" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AH38" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AI38" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:40" ht="24" customHeight="1">
+      <c r="A40" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="41" spans="1:40" ht="24" customHeight="1">
+      <c r="A41" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40" ht="24" customHeight="1">
+      <c r="B42" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
-      <c r="AA31" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="AB31" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="AC31" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="AD31" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:40" ht="24" customHeight="1">
-      <c r="A33" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="34" spans="1:40" ht="24" customHeight="1">
-      <c r="A34" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="35" spans="1:40" ht="24" customHeight="1">
-      <c r="B35" s="10" t="s">
+    <row r="43" spans="1:40" ht="24" customHeight="1">
+      <c r="B43" s="11"/>
+      <c r="AA43" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="AB43" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="AC43" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="AD43" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:40" ht="24" customHeight="1">
+      <c r="A45" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="46" spans="1:40" ht="24" customHeight="1">
+      <c r="A46" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="47" spans="1:40" ht="24" customHeight="1">
+      <c r="B47" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="24" customHeight="1">
-      <c r="B36" s="11"/>
-      <c r="AA36" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="AB36" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="AC36" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="AD36" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="AE36" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="AF36" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="AG36" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="AH36" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="AI36" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="AJ36" s="6" t="s">
+    <row r="48" spans="1:40" ht="24" customHeight="1">
+      <c r="B48" s="11"/>
+      <c r="AA48" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="AK36" s="6" t="s">
+      <c r="AB48" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="AL36" s="6" t="s">
+      <c r="AC48" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="AM36" s="6" t="s">
+      <c r="AD48" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="AE48" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="AN36" s="6" t="s">
-        <v>65</v>
+      <c r="AF48" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="AG48" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="AH48" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="AI48" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="AJ48" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AK48" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="AL48" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="AM48" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="AN48" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="17">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
       <formula1>AA16:AM16</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+      <formula1>AA17:AM17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
+      <formula1>AA18:AM18</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
+      <formula1>AA19:AM19</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+      <formula1>AA20:AM20</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
-      <formula1>AA21:AH21</formula1>
+      <formula1>AA21:AM21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26">
-      <formula1>AA26:AI26</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
+      <formula1>AA22:AM22</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
+      <formula1>AA23:AM23</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+      <formula1>AA24:AM24</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
+      <formula1>AA25:AM25</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
+      <formula1>AA30:AH30</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
-      <formula1>AA31:AD31</formula1>
+      <formula1>AA31:AH31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36">
-      <formula1>AA36:AN36</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
+      <formula1>AA32:AH32</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
+      <formula1>AA37:AI37</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
+      <formula1>AA38:AI38</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43">
+      <formula1>AA43:AD43</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48">
+      <formula1>AA48:AN48</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>